<commit_message>
changed get_involved route to get-involved
</commit_message>
<xml_diff>
--- a/src/assets/downloads/OpenEnzymeDatabase-ContributionTemplate-1.0.0.xlsx
+++ b/src/assets/downloads/OpenEnzymeDatabase-ContributionTemplate-1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjberry/Projects/OpenEnzymeDB-frontend/src/assets/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C76FACEC-49B6-0640-99D2-34F10ECE392B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9389A9E-E1C0-1A4E-90A4-3D77E65125CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12760" yWindow="9840" windowWidth="26180" windowHeight="15860" xr2:uid="{A211E642-6450-B943-8DAE-4028FCB8D425}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Open Enzyme Database</t>
   </si>
   <si>
-    <t>To upload your completed form, follow the instructions at https://openenzymedb.platform.moleculemaker.org/about/get_involved.</t>
-  </si>
-  <si>
     <t>For any questions or suggestions, please email us at oed-feedback@moleculemaker.org.</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
       </rPr>
       <t xml:space="preserve"> - On this tab, please enter the data you would like to contribute to the OED. Note the fields for each type of kinetic data correspond to the column headsing of the experimental data tables in the OED, with the same units.</t>
     </r>
+  </si>
+  <si>
+    <t>To upload your completed form, follow the instructions at https://openenzymedb.platform.moleculemaker.org/about/get-involved.</t>
   </si>
 </sst>
 </file>
@@ -237,11 +237,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -598,67 +597,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="28" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-    </row>
-    <row r="6" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="9" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="11" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-    </row>
-    <row r="13" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
     </row>
     <row r="16" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>4</v>
+      <c r="A16" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -684,27 +683,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -724,57 +723,55 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="3"/>
-    <col min="8" max="8" width="13.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13" style="3" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>